<commit_message>
Added new sampled training scripts + models
</commit_message>
<xml_diff>
--- a/DatasetBalance.xlsx
+++ b/DatasetBalance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SARRAA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60E869B-2230-48DF-B8EB-C6913A92FF2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A28C2B-DA27-49DB-8B4F-408EE9BCD447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D57376AF-35EC-476A-BFA6-F03FEED75E10}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Benign</t>
   </si>
@@ -72,6 +72,15 @@
   </si>
   <si>
     <t>11.411 - 33.83 %</t>
+  </si>
+  <si>
+    <t>sqli fixed reduced balanced</t>
+  </si>
+  <si>
+    <t>11.455 - 50.08 %</t>
+  </si>
+  <si>
+    <t>11411 - 49.92 %</t>
   </si>
 </sst>
 </file>
@@ -138,7 +147,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -208,6 +217,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -215,60 +233,90 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="4" borderId="7" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="3" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -588,143 +636,174 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1B148E0-50F7-49AB-993A-D99E18E24052}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W14" sqref="W14:W15"/>
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="23" customWidth="1"/>
     <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="7" max="7" width="31.5703125" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="22"/>
+      <c r="J1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2"/>
+      <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="22"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="5" t="s">
+      <c r="D3" s="11"/>
+      <c r="E3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="H3" s="5" t="s">
+      <c r="F3" s="11"/>
+      <c r="G3" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="19"/>
+      <c r="J3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="6"/>
+      <c r="K3" s="11"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="8"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="8"/>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="19"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="13"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="9" t="s">
+      <c r="B5" s="18"/>
+      <c r="C5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="9" t="s">
+      <c r="D5" s="15"/>
+      <c r="E5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="H5" s="9" t="s">
+      <c r="F5" s="15"/>
+      <c r="G5" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="20"/>
+      <c r="J5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="10"/>
+      <c r="K5" s="15"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="12"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="12"/>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="20"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="17"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="15">
+      <c r="B8" s="4"/>
+      <c r="C8" s="6">
         <v>16405</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="15">
+      <c r="D8" s="7"/>
+      <c r="E8" s="6">
         <v>33716</v>
       </c>
-      <c r="F8" s="16"/>
-      <c r="H8" s="15">
+      <c r="F8" s="7"/>
+      <c r="G8" s="26">
+        <v>22866</v>
+      </c>
+      <c r="H8" s="21"/>
+      <c r="J8" s="6">
         <v>50121</v>
       </c>
-      <c r="I8" s="16"/>
+      <c r="K8" s="7"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="18"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="18"/>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="21"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="20">
+    <mergeCell ref="J1:K2"/>
+    <mergeCell ref="J3:K4"/>
+    <mergeCell ref="J5:K6"/>
+    <mergeCell ref="J8:K9"/>
+    <mergeCell ref="C3:D4"/>
+    <mergeCell ref="E3:F4"/>
+    <mergeCell ref="C5:D6"/>
+    <mergeCell ref="E5:F6"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="G8:G9"/>
     <mergeCell ref="C1:D2"/>
     <mergeCell ref="E1:F2"/>
     <mergeCell ref="A8:B9"/>
     <mergeCell ref="C8:D9"/>
     <mergeCell ref="E8:F9"/>
-    <mergeCell ref="H1:I2"/>
-    <mergeCell ref="H3:I4"/>
-    <mergeCell ref="H5:I6"/>
-    <mergeCell ref="H8:I9"/>
-    <mergeCell ref="C3:D4"/>
-    <mergeCell ref="E3:F4"/>
-    <mergeCell ref="C5:D6"/>
-    <mergeCell ref="E5:F6"/>
     <mergeCell ref="A3:B4"/>
     <mergeCell ref="A5:B6"/>
   </mergeCells>

</xml_diff>